<commit_message>
Small update of input and buymodel dictionary for testing purposes.
</commit_message>
<xml_diff>
--- a/dictionary/buymodel.xlsx
+++ b/dictionary/buymodel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6531BD6F-76C3-4ECB-AE86-50DEB572FAB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE5E81E-35D6-414D-B6B7-60048D36C61E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Buy Model</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Vendor</t>
+  </si>
+  <si>
+    <t>ad4games</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +750,7 @@
         <v>30</v>
       </c>
       <c r="C27">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -758,7 +761,7 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>3.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -769,7 +772,7 @@
         <v>30</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,7 +783,7 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -791,7 +794,18 @@
         <v>30</v>
       </c>
       <c r="C31">
-        <v>4.2</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality: - possibility to add Start and End Date - optional: one or both Dates can be left blank
</commit_message>
<xml_diff>
--- a/dictionary/buymodel.xlsx
+++ b/dictionary/buymodel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE5E81E-35D6-414D-B6B7-60048D36C61E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664105D1-7BA7-4571-9133-28D14D278E04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,7 +127,7 @@
     <t>Vendor</t>
   </si>
   <si>
-    <t>ad4games</t>
+    <t>ad4game</t>
   </si>
 </sst>
 </file>

</xml_diff>